<commit_message>
Implementacion temporal de GLOSAS CARGUE
</commit_message>
<xml_diff>
--- a/static/FORMAT_GLOSA.xlsx
+++ b/static/FORMAT_GLOSA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LUIS CARLOS VASQUEZ TORO\ProyectosElectron\Fact.Squid\static\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\ProyectosElectron\Fact.Squid\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="GLOSAS" sheetId="1" r:id="rId1"/>
+    <sheet name="DETAILS" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">FECHA_DE_GLOSA </t>
   </si>
@@ -42,14 +43,76 @@
   </si>
   <si>
     <t>FACTURA</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>TIPO DE CARGA</t>
+  </si>
+  <si>
+    <t>MANUAL</t>
+  </si>
+  <si>
+    <t>HUB</t>
+  </si>
+  <si>
+    <t>Fact.Squid</t>
+  </si>
+  <si>
+    <t>DOCUMENTO GESTOR</t>
+  </si>
+  <si>
+    <t>FECHA DOCUMENTO</t>
+  </si>
+  <si>
+    <t>TIPO</t>
+  </si>
+  <si>
+    <t>TIPOS</t>
+  </si>
+  <si>
+    <t>1-GLOSA_RATIFICADA</t>
+  </si>
+  <si>
+    <t>0-GLOSA_INICIAL</t>
+  </si>
+  <si>
+    <t>2-GLOSA_INICIAL_SALDO_CERO</t>
+  </si>
+  <si>
+    <t>3-GLOSA_RATIFICADA_SALDO_CERO</t>
+  </si>
+  <si>
+    <t>4-DEVOLUCION</t>
+  </si>
+  <si>
+    <t>5-FACTURA_DEVUELTA(GLOSA 100%)</t>
+  </si>
+  <si>
+    <t>6-FACTURA_DEVUELTA(NO_ACEPTACION)</t>
+  </si>
+  <si>
+    <t>NIT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -73,13 +136,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,40 +454,180 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>DETAILS!$B$5:$B$11</xm:f>
+          </x14:formula1>
+          <xm:sqref>B3</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>